<commit_message>
sullivan.py captures the requirement for a set of four terminal-pair measurements of a set of inductors. Only a coaxial zero is needed to correct for the bridge. There are no device dependent zero definitions.
</commit_message>
<xml_diff>
--- a/sullivan_Results.xlsx
+++ b/sullivan_Results.xlsx
@@ -439,13 +439,13 @@
         <v>-1</v>
       </c>
       <c r="E2" t="n">
-        <v>-10</v>
+        <v>-6</v>
       </c>
       <c r="F2" t="n">
-        <v>1592.12</v>
+        <v>1593.07</v>
       </c>
       <c r="G2" t="n">
-        <v>20</v>
+        <v>19.71</v>
       </c>
       <c r="H2" t="n">
         <v>0.5</v>
@@ -490,10 +490,10 @@
         <v>0</v>
       </c>
       <c r="V2" t="n">
-        <v>1.256186719711855e-08</v>
+        <v>1.255437614258792e-08</v>
       </c>
       <c r="W2" t="n">
-        <v>0.0001256186719711845</v>
+        <v>0.0001255437614234308</v>
       </c>
     </row>
     <row r="3">
@@ -511,16 +511,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>99399</v>
+        <v>99380</v>
       </c>
       <c r="E3" t="n">
-        <v>569099</v>
+        <v>569169</v>
       </c>
       <c r="F3" t="n">
-        <v>1592.22</v>
+        <v>1593.33</v>
       </c>
       <c r="G3" t="n">
-        <v>20</v>
+        <v>19.73</v>
       </c>
       <c r="H3" t="n">
         <v>0.5</v>
@@ -547,28 +547,28 @@
         <v>10</v>
       </c>
       <c r="P3" t="n">
-        <v>0.0009942049713033017</v>
+        <v>0.0009940168196829501</v>
       </c>
       <c r="Q3" t="n">
-        <v>6.268122824340361e-08</v>
+        <v>6.321253794347984e-08</v>
       </c>
       <c r="R3" t="n">
-        <v>1.989878160259134</v>
+        <v>1.988966074789402</v>
       </c>
       <c r="S3" t="n">
-        <v>5.691499194643115</v>
+        <v>5.68601177492092</v>
       </c>
       <c r="T3" t="n">
-        <v>0.03371038803545611</v>
+        <v>0.03371896508567265</v>
       </c>
       <c r="U3" t="n">
-        <v>2.083526072462429</v>
+        <v>2.08343460112531</v>
       </c>
       <c r="V3" t="n">
-        <v>1.959346177075566e-08</v>
+        <v>1.958623812165344e-08</v>
       </c>
       <c r="W3" t="n">
-        <v>0.0001789165779757623</v>
+        <v>0.000178849360134071</v>
       </c>
     </row>
     <row r="4">
@@ -586,16 +586,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>198037</v>
+        <v>198010</v>
       </c>
       <c r="E4" t="n">
-        <v>838177</v>
+        <v>838356</v>
       </c>
       <c r="F4" t="n">
-        <v>1592.31</v>
+        <v>1593.46</v>
       </c>
       <c r="G4" t="n">
-        <v>20</v>
+        <v>19.71</v>
       </c>
       <c r="H4" t="n">
         <v>0.5</v>
@@ -622,28 +622,28 @@
         <v>10</v>
       </c>
       <c r="P4" t="n">
-        <v>0.001980788371297418</v>
+        <v>0.001980521284213081</v>
       </c>
       <c r="Q4" t="n">
-        <v>9.716764875291919e-08</v>
+        <v>9.853466689660475e-08</v>
       </c>
       <c r="R4" t="n">
-        <v>2.002360736055591</v>
+        <v>2.000304638636801</v>
       </c>
       <c r="S4" t="n">
-        <v>8.382472664217801</v>
+        <v>8.374497161212975</v>
       </c>
       <c r="T4" t="n">
-        <v>0.04957231347915256</v>
+        <v>0.04959054289304366</v>
       </c>
       <c r="U4" t="n">
-        <v>2.08460840255336</v>
+        <v>2.084499826805902</v>
       </c>
       <c r="V4" t="n">
-        <v>3.157577679572181e-08</v>
+        <v>3.156950443102184e-08</v>
       </c>
       <c r="W4" t="n">
-        <v>0.0002622649274586944</v>
+        <v>0.0002622134371218887</v>
       </c>
     </row>
     <row r="5">
@@ -661,16 +661,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>296910</v>
+        <v>296879</v>
       </c>
       <c r="E5" t="n">
-        <v>1066102</v>
+        <v>1066481</v>
       </c>
       <c r="F5" t="n">
-        <v>1592.41</v>
+        <v>1593.67</v>
       </c>
       <c r="G5" t="n">
-        <v>20</v>
+        <v>19.71</v>
       </c>
       <c r="H5" t="n">
         <v>0.5</v>
@@ -697,28 +697,28 @@
         <v>10</v>
       </c>
       <c r="P5" t="n">
-        <v>0.002969722255881637</v>
+        <v>0.002969416642769562</v>
       </c>
       <c r="Q5" t="n">
-        <v>1.361128123695792e-07</v>
+        <v>1.382915076109563e-07</v>
       </c>
       <c r="R5" t="n">
-        <v>2.013207068580783</v>
+        <v>2.010169515041158</v>
       </c>
       <c r="S5" t="n">
-        <v>10.66188654440425</v>
+        <v>10.65326474493345</v>
       </c>
       <c r="T5" t="n">
-        <v>0.06302173832542715</v>
+        <v>0.0630539012780922</v>
       </c>
       <c r="U5" t="n">
-        <v>2.084953310471516</v>
+        <v>2.084843858322008</v>
       </c>
       <c r="V5" t="n">
-        <v>4.472111514854902e-08</v>
+        <v>4.471547759106351e-08</v>
       </c>
       <c r="W5" t="n">
-        <v>0.0003553114916579031</v>
+        <v>0.0003552745963425761</v>
       </c>
     </row>
     <row r="6">
@@ -736,16 +736,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>394862</v>
+        <v>394832</v>
       </c>
       <c r="E6" t="n">
-        <v>1264597</v>
+        <v>1265232</v>
       </c>
       <c r="F6" t="n">
-        <v>1592.51</v>
+        <v>1593.74</v>
       </c>
       <c r="G6" t="n">
-        <v>20</v>
+        <v>19.7</v>
       </c>
       <c r="H6" t="n">
         <v>0.5</v>
@@ -772,28 +772,28 @@
         <v>10</v>
       </c>
       <c r="P6" t="n">
-        <v>0.003949444241285067</v>
+        <v>0.003949149308890628</v>
       </c>
       <c r="Q6" t="n">
-        <v>1.760463415605935e-07</v>
+        <v>1.790148686677638e-07</v>
       </c>
       <c r="R6" t="n">
-        <v>2.019349139974328</v>
+        <v>2.015710172132742</v>
       </c>
       <c r="S6" t="n">
-        <v>12.64697926414807</v>
+        <v>12.63810584218668</v>
       </c>
       <c r="T6" t="n">
-        <v>0.07473950745286334</v>
+        <v>0.07478944908286286</v>
       </c>
       <c r="U6" t="n">
-        <v>2.085106232410725</v>
+        <v>2.084988667016243</v>
       </c>
       <c r="V6" t="n">
-        <v>5.809372445490924e-08</v>
+        <v>5.80893985225214e-08</v>
       </c>
       <c r="W6" t="n">
-        <v>0.0004506679127728641</v>
+        <v>0.0004506520815701664</v>
       </c>
     </row>
     <row r="7">
@@ -811,16 +811,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>493235</v>
+        <v>493210</v>
       </c>
       <c r="E7" t="n">
-        <v>1441386</v>
+        <v>1442337</v>
       </c>
       <c r="F7" t="n">
-        <v>1592.6</v>
+        <v>1592.85</v>
       </c>
       <c r="G7" t="n">
-        <v>20</v>
+        <v>19.71</v>
       </c>
       <c r="H7" t="n">
         <v>0.5</v>
@@ -847,28 +847,28 @@
         <v>10</v>
       </c>
       <c r="P7" t="n">
-        <v>0.004933377094826513</v>
+        <v>0.00493313443743475</v>
       </c>
       <c r="Q7" t="n">
-        <v>2.166892527540896e-07</v>
+        <v>2.204442596719743e-07</v>
       </c>
       <c r="R7" t="n">
-        <v>2.023089443234102</v>
+        <v>2.019069475039879</v>
       </c>
       <c r="S7" t="n">
-        <v>14.41499637707681</v>
+        <v>14.40773474579633</v>
       </c>
       <c r="T7" t="n">
-        <v>0.08517856014088322</v>
+        <v>0.08524795306321042</v>
       </c>
       <c r="U7" t="n">
-        <v>2.085185008267143</v>
+        <v>2.08507527367559</v>
       </c>
       <c r="V7" t="n">
-        <v>7.166424750046625e-08</v>
+        <v>7.166292781028802e-08</v>
       </c>
       <c r="W7" t="n">
-        <v>0.0005476114858144654</v>
+        <v>0.0005476367680598177</v>
       </c>
     </row>
     <row r="8">
@@ -886,16 +886,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>591477</v>
+        <v>591464</v>
       </c>
       <c r="E8" t="n">
-        <v>1609922</v>
+        <v>1611164</v>
       </c>
       <c r="F8" t="n">
-        <v>1592.68</v>
+        <v>1592.97</v>
       </c>
       <c r="G8" t="n">
-        <v>20</v>
+        <v>19.7</v>
       </c>
       <c r="H8" t="n">
         <v>0.5</v>
@@ -922,28 +922,28 @@
         <v>10</v>
       </c>
       <c r="P8" t="n">
-        <v>0.005915999678234755</v>
+        <v>0.005915877335408122</v>
       </c>
       <c r="Q8" t="n">
-        <v>2.576026042419898e-07</v>
+        <v>2.621421023954124e-07</v>
       </c>
       <c r="R8" t="n">
-        <v>2.025477092515757</v>
+        <v>2.021207037917273</v>
       </c>
       <c r="S8" t="n">
-        <v>16.1004775560221</v>
+        <v>16.09352308802535</v>
       </c>
       <c r="T8" t="n">
-        <v>0.09513181097846164</v>
+        <v>0.09522098677452703</v>
       </c>
       <c r="U8" t="n">
-        <v>2.085232679216086</v>
+        <v>2.085115084871771</v>
       </c>
       <c r="V8" t="n">
-        <v>8.530359166213372e-08</v>
+        <v>8.530441989505636e-08</v>
       </c>
       <c r="W8" t="n">
-        <v>0.0006454191174672897</v>
+        <v>0.0006454674611146695</v>
       </c>
     </row>
     <row r="9">
@@ -961,16 +961,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>689150</v>
+        <v>689154</v>
       </c>
       <c r="E9" t="n">
-        <v>1774172</v>
+        <v>1775693</v>
       </c>
       <c r="F9" t="n">
-        <v>1592.75</v>
+        <v>1593.08</v>
       </c>
       <c r="G9" t="n">
-        <v>20</v>
+        <v>19.7</v>
       </c>
       <c r="H9" t="n">
         <v>0.5</v>
@@ -997,28 +997,28 @@
         <v>10</v>
       </c>
       <c r="P9" t="n">
-        <v>0.006892931088316318</v>
+        <v>0.006892980049668741</v>
       </c>
       <c r="Q9" t="n">
-        <v>2.98480680408779e-07</v>
+        <v>3.03798234077337e-07</v>
       </c>
       <c r="R9" t="n">
-        <v>2.027080136210438</v>
+        <v>2.022640790532277</v>
       </c>
       <c r="S9" t="n">
-        <v>17.74309565329367</v>
+        <v>17.73695689594307</v>
       </c>
       <c r="T9" t="n">
-        <v>0.1048329338407019</v>
+        <v>0.1049402095214556</v>
       </c>
       <c r="U9" t="n">
-        <v>2.085263721102124</v>
+        <v>2.085146043611084</v>
       </c>
       <c r="V9" t="n">
-        <v>9.891871596893705e-08</v>
+        <v>9.892234889453298e-08</v>
       </c>
       <c r="W9" t="n">
-        <v>0.0007433671395705812</v>
+        <v>0.0007434423086112874</v>
       </c>
     </row>
     <row r="10">
@@ -1036,16 +1036,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>786374</v>
+        <v>786400</v>
       </c>
       <c r="E10" t="n">
-        <v>1925612</v>
+        <v>1927498</v>
       </c>
       <c r="F10" t="n">
-        <v>1592.85</v>
+        <v>1593.25</v>
       </c>
       <c r="G10" t="n">
-        <v>20</v>
+        <v>19.69</v>
       </c>
       <c r="H10" t="n">
         <v>0.5</v>
@@ -1072,28 +1072,28 @@
         <v>10</v>
       </c>
       <c r="P10" t="n">
-        <v>0.007865371572521471</v>
+        <v>0.007865640269459415</v>
       </c>
       <c r="Q10" t="n">
-        <v>3.392405401427413e-07</v>
+        <v>3.453360394319712e-07</v>
       </c>
       <c r="R10" t="n">
-        <v>2.02826092953414</v>
+        <v>2.023693546726142</v>
       </c>
       <c r="S10" t="n">
-        <v>19.25760454005659</v>
+        <v>19.25252319952976</v>
       </c>
       <c r="T10" t="n">
-        <v>0.113778499925359</v>
+        <v>0.1139101160682761</v>
       </c>
       <c r="U10" t="n">
-        <v>2.08528113508035</v>
+        <v>2.085155411240929</v>
       </c>
       <c r="V10" t="n">
-        <v>1.124892628582008e-07</v>
+        <v>1.124964921201696e-07</v>
       </c>
       <c r="W10" t="n">
-        <v>0.0008408873924082658</v>
+        <v>0.0008409970778318691</v>
       </c>
     </row>
     <row r="11">
@@ -1111,16 +1111,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>883275</v>
+        <v>883362</v>
       </c>
       <c r="E11" t="n">
-        <v>2071149</v>
+        <v>2073610</v>
       </c>
       <c r="F11" t="n">
-        <v>1592.92</v>
+        <v>1593.16</v>
       </c>
       <c r="G11" t="n">
-        <v>20</v>
+        <v>19.7</v>
       </c>
       <c r="H11" t="n">
         <v>0.5</v>
@@ -1147,28 +1147,28 @@
         <v>10</v>
       </c>
       <c r="P11" t="n">
-        <v>0.00883458139067299</v>
+        <v>0.00883546304619987</v>
       </c>
       <c r="Q11" t="n">
-        <v>3.799339086869312e-07</v>
+        <v>3.868176692643267e-07</v>
       </c>
       <c r="R11" t="n">
-        <v>2.029148854283147</v>
+        <v>2.024487040268303</v>
       </c>
       <c r="S11" t="n">
-        <v>20.71307918250781</v>
+        <v>20.71276583997981</v>
       </c>
       <c r="T11" t="n">
-        <v>0.1223760485398487</v>
+        <v>0.1225417546724499</v>
       </c>
       <c r="U11" t="n">
-        <v>2.085291557544155</v>
+        <v>2.085173993463791</v>
       </c>
       <c r="V11" t="n">
-        <v>1.260333339608992e-07</v>
+        <v>1.260500337935669e-07</v>
       </c>
       <c r="W11" t="n">
-        <v>0.000938269743719769</v>
+        <v>0.000938461759000262</v>
       </c>
     </row>
     <row r="12">
@@ -1186,16 +1186,16 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>980309</v>
+        <v>980451</v>
       </c>
       <c r="E12" t="n">
-        <v>2218833</v>
+        <v>2222585</v>
       </c>
       <c r="F12" t="n">
-        <v>1591.29</v>
+        <v>1592.88</v>
       </c>
       <c r="G12" t="n">
-        <v>20</v>
+        <v>19.86</v>
       </c>
       <c r="H12" t="n">
         <v>0.5</v>
@@ -1222,28 +1222,28 @@
         <v>10</v>
       </c>
       <c r="P12" t="n">
-        <v>0.009805121483081889</v>
+        <v>0.009806585894470006</v>
       </c>
       <c r="Q12" t="n">
-        <v>4.20766781295227e-07</v>
+        <v>4.284138567750588e-07</v>
       </c>
       <c r="R12" t="n">
-        <v>2.029816423247701</v>
+        <v>2.025100348748243</v>
       </c>
       <c r="S12" t="n">
-        <v>22.19002536867193</v>
+        <v>22.2150606926055</v>
       </c>
       <c r="T12" t="n">
-        <v>0.1311005662416511</v>
+        <v>0.1313269406267873</v>
       </c>
       <c r="U12" t="n">
-        <v>2.085300001355345</v>
+        <v>2.085274685471221</v>
       </c>
       <c r="V12" t="n">
-        <v>1.396203399884707e-07</v>
+        <v>1.396457138224739e-07</v>
       </c>
       <c r="W12" t="n">
-        <v>0.001036198636538412</v>
+        <v>0.001036482195090958</v>
       </c>
     </row>
     <row r="13">
@@ -1261,16 +1261,16 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>99137</v>
+        <v>99118</v>
       </c>
       <c r="E13" t="n">
-        <v>1166002</v>
+        <v>1166562</v>
       </c>
       <c r="F13" t="n">
-        <v>1591.73</v>
+        <v>1594.81</v>
       </c>
       <c r="G13" t="n">
-        <v>20</v>
+        <v>19.77</v>
       </c>
       <c r="H13" t="n">
         <v>0.5</v>
@@ -1297,28 +1297,28 @@
         <v>10</v>
       </c>
       <c r="P13" t="n">
-        <v>9.915944330989743e-05</v>
+        <v>9.914170718239515e-05</v>
       </c>
       <c r="Q13" t="n">
-        <v>7.168147349062037e-09</v>
+        <v>7.21351138133991e-09</v>
       </c>
       <c r="R13" t="n">
-        <v>1.998599486761582</v>
+        <v>1.997657557397754</v>
       </c>
       <c r="S13" t="n">
-        <v>1.166100837702475</v>
+        <v>1.165597564479266</v>
       </c>
       <c r="T13" t="n">
-        <v>0.006891134402591001</v>
+        <v>0.006895113510952668</v>
       </c>
       <c r="U13" t="n">
-        <v>2.085117281712405</v>
+        <v>2.085048485178118</v>
       </c>
       <c r="V13" t="n">
-        <v>2.205820827808296e-09</v>
+        <v>2.204574624214287e-09</v>
       </c>
       <c r="W13" t="n">
-        <v>2.286289658237565e-05</v>
+        <v>2.285437881499195e-05</v>
       </c>
     </row>
     <row r="14">
@@ -1336,16 +1336,16 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>198991</v>
+        <v>198956</v>
       </c>
       <c r="E14" t="n">
-        <v>1738805</v>
+        <v>1739697</v>
       </c>
       <c r="F14" t="n">
-        <v>1591.79</v>
+        <v>1594.95</v>
       </c>
       <c r="G14" t="n">
-        <v>20</v>
+        <v>19.76</v>
       </c>
       <c r="H14" t="n">
         <v>0.5</v>
@@ -1372,28 +1372,28 @@
         <v>10</v>
       </c>
       <c r="P14" t="n">
-        <v>0.0001990340340589115</v>
+        <v>0.0001990005243383183</v>
       </c>
       <c r="Q14" t="n">
-        <v>1.104330158966115e-08</v>
+        <v>1.11644392449385e-08</v>
       </c>
       <c r="R14" t="n">
-        <v>2.00458607733815</v>
+        <v>2.002804983453184</v>
       </c>
       <c r="S14" t="n">
-        <v>1.738945022768809</v>
+        <v>1.738176858421052</v>
       </c>
       <c r="T14" t="n">
-        <v>0.01027255783653466</v>
+        <v>0.01027892336698842</v>
       </c>
       <c r="U14" t="n">
-        <v>2.085385833603788</v>
+        <v>2.085310073182456</v>
       </c>
       <c r="V14" t="n">
-        <v>3.516650697589006e-09</v>
+        <v>3.515831111854671e-09</v>
       </c>
       <c r="W14" t="n">
-        <v>3.386271490046173e-05</v>
+        <v>3.38604964230146e-05</v>
       </c>
     </row>
     <row r="15">
@@ -1411,16 +1411,16 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>298239</v>
+        <v>298184</v>
       </c>
       <c r="E15" t="n">
-        <v>2205906</v>
+        <v>2207103</v>
       </c>
       <c r="F15" t="n">
-        <v>1591.84</v>
+        <v>1595.08</v>
       </c>
       <c r="G15" t="n">
-        <v>20</v>
+        <v>19.75</v>
       </c>
       <c r="H15" t="n">
         <v>0.5</v>
@@ -1447,28 +1447,28 @@
         <v>10</v>
       </c>
       <c r="P15" t="n">
-        <v>0.0002983024998455413</v>
+        <v>0.0002982491743606949</v>
       </c>
       <c r="Q15" t="n">
-        <v>1.512921894769727e-08</v>
+        <v>1.532759379682069e-08</v>
       </c>
       <c r="R15" t="n">
-        <v>2.008910512481534</v>
+        <v>2.006586444293072</v>
       </c>
       <c r="S15" t="n">
-        <v>2.206079607763423</v>
+        <v>2.20507943285509</v>
       </c>
       <c r="T15" t="n">
-        <v>0.01303064788325398</v>
+        <v>0.01303923098466725</v>
       </c>
       <c r="U15" t="n">
-        <v>2.0854659580206</v>
+        <v>2.085383461903509</v>
       </c>
       <c r="V15" t="n">
-        <v>4.887329142352857e-09</v>
+        <v>4.886582170902018e-09</v>
       </c>
       <c r="W15" t="n">
-        <v>4.47388559400525e-05</v>
+        <v>4.473974635527407e-05</v>
       </c>
     </row>
     <row r="16">
@@ -1486,16 +1486,16 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>396505</v>
+        <v>396438</v>
       </c>
       <c r="E16" t="n">
-        <v>2790983</v>
+        <v>2792679</v>
       </c>
       <c r="F16" t="n">
-        <v>1591.91</v>
+        <v>1595.22</v>
       </c>
       <c r="G16" t="n">
-        <v>20</v>
+        <v>19.74</v>
       </c>
       <c r="H16" t="n">
         <v>0.5</v>
@@ -1522,28 +1522,28 @@
         <v>10</v>
       </c>
       <c r="P16" t="n">
-        <v>0.0003965887631353706</v>
+        <v>0.0003965235817915425</v>
       </c>
       <c r="Q16" t="n">
-        <v>1.953538064497496e-08</v>
+        <v>1.980695884882506e-08</v>
       </c>
       <c r="R16" t="n">
-        <v>2.01208783252256</v>
+        <v>2.009449846405277</v>
       </c>
       <c r="S16" t="n">
-        <v>2.791198675341726</v>
+        <v>2.790000203016651</v>
       </c>
       <c r="T16" t="n">
-        <v>0.01648562669715748</v>
+        <v>0.01649771681718106</v>
       </c>
       <c r="U16" t="n">
-        <v>2.085516576489306</v>
+        <v>2.085427176881368</v>
       </c>
       <c r="V16" t="n">
-        <v>6.340048546247283e-09</v>
+        <v>6.339493352381419e-09</v>
       </c>
       <c r="W16" t="n">
-        <v>5.707566191019419e-05</v>
+        <v>5.708173665713881e-05</v>
       </c>
     </row>
     <row r="17">
@@ -1561,16 +1561,16 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>494440</v>
+        <v>494367</v>
       </c>
       <c r="E17" t="n">
-        <v>3174124</v>
+        <v>3176412</v>
       </c>
       <c r="F17" t="n">
-        <v>1591.99</v>
+        <v>1.59532</v>
       </c>
       <c r="G17" t="n">
-        <v>20</v>
+        <v>19.71</v>
       </c>
       <c r="H17" t="n">
         <v>0.5</v>
@@ -1597,28 +1597,28 @@
         <v>10</v>
       </c>
       <c r="P17" t="n">
-        <v>0.0004945439581701683</v>
+        <v>0.0004944726844883379</v>
       </c>
       <c r="Q17" t="n">
-        <v>2.366698318120194e-08</v>
+        <v>3.643750200513162e-07</v>
       </c>
       <c r="R17" t="n">
-        <v>2.013905283491961</v>
+        <v>2.224972110923106</v>
       </c>
       <c r="S17" t="n">
-        <v>3.174367223534561</v>
+        <v>3.172980485914009</v>
       </c>
       <c r="T17" t="n">
-        <v>0.01874832601823212</v>
+        <v>0.01899651737571835</v>
       </c>
       <c r="U17" t="n">
-        <v>2.08553249648875</v>
+        <v>2.077405926595824</v>
       </c>
       <c r="V17" t="n">
-        <v>7.719510181214619e-09</v>
+        <v>1.253690113276088e-06</v>
       </c>
       <c r="W17" t="n">
-        <v>6.766491053895208e-05</v>
+        <v>0.01253684615535567</v>
       </c>
     </row>
     <row r="18">
@@ -1636,16 +1636,16 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>593475</v>
+        <v>593385</v>
       </c>
       <c r="E18" t="n">
-        <v>3537225</v>
+        <v>3538125</v>
       </c>
       <c r="F18" t="n">
-        <v>1591.64</v>
+        <v>1594.66</v>
       </c>
       <c r="G18" t="n">
-        <v>20</v>
+        <v>19.77</v>
       </c>
       <c r="H18" t="n">
         <v>0.5</v>
@@ -1672,28 +1672,28 @@
         <v>10</v>
       </c>
       <c r="P18" t="n">
-        <v>0.000593599380034376</v>
+        <v>0.0005935119635064693</v>
       </c>
       <c r="Q18" t="n">
-        <v>2.786419176217035e-08</v>
+        <v>2.828718412968693e-08</v>
       </c>
       <c r="R18" t="n">
-        <v>2.015463419717579</v>
+        <v>2.012382810330637</v>
       </c>
       <c r="S18" t="n">
-        <v>3.537494330832831</v>
+        <v>3.535149087219765</v>
       </c>
       <c r="T18" t="n">
-        <v>0.02089274688253611</v>
+        <v>0.02090012160625787</v>
       </c>
       <c r="U18" t="n">
-        <v>2.085541974774175</v>
+        <v>2.085471843265076</v>
       </c>
       <c r="V18" t="n">
-        <v>9.118928414290208e-09</v>
+        <v>9.117856782426842e-09</v>
       </c>
       <c r="W18" t="n">
-        <v>7.83209496367488e-05</v>
+        <v>7.831861045648451e-05</v>
       </c>
     </row>
     <row r="19">
@@ -1711,16 +1711,16 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>691294</v>
+        <v>691195</v>
       </c>
       <c r="E19" t="n">
-        <v>3889800</v>
+        <v>3896072</v>
       </c>
       <c r="F19" t="n">
-        <v>1592.21</v>
+        <v>1594.9</v>
       </c>
       <c r="G19" t="n">
-        <v>20</v>
+        <v>19.78</v>
       </c>
       <c r="H19" t="n">
         <v>0.5</v>
@@ -1747,28 +1747,28 @@
         <v>10</v>
       </c>
       <c r="P19" t="n">
-        <v>0.0006914385511489813</v>
+        <v>0.0006913425350652059</v>
       </c>
       <c r="Q19" t="n">
-        <v>3.203715260404981e-08</v>
+        <v>3.254298181867987e-08</v>
       </c>
       <c r="R19" t="n">
-        <v>2.016737707297789</v>
+        <v>2.013491670048263</v>
       </c>
       <c r="S19" t="n">
-        <v>3.890094681301949</v>
+        <v>3.892948343108125</v>
       </c>
       <c r="T19" t="n">
-        <v>0.02297504793072487</v>
+        <v>0.02301416172059972</v>
       </c>
       <c r="U19" t="n">
-        <v>2.085548078510993</v>
+        <v>2.085484093773392</v>
       </c>
       <c r="V19" t="n">
-        <v>1.050785940751035e-08</v>
+        <v>1.05087183821401e-08</v>
       </c>
       <c r="W19" t="n">
-        <v>8.890804693338038e-05</v>
+        <v>8.895157222589057e-05</v>
       </c>
     </row>
     <row r="20">
@@ -1786,16 +1786,16 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>789069</v>
+        <v>788963</v>
       </c>
       <c r="E20" t="n">
-        <v>4192210</v>
+        <v>4199748</v>
       </c>
       <c r="F20" t="n">
-        <v>1592.28</v>
+        <v>1595.1</v>
       </c>
       <c r="G20" t="n">
-        <v>20</v>
+        <v>19.79</v>
       </c>
       <c r="H20" t="n">
         <v>0.5</v>
@@ -1822,28 +1822,28 @@
         <v>10</v>
       </c>
       <c r="P20" t="n">
-        <v>0.0007892337131904102</v>
+        <v>0.0007891311369653564</v>
       </c>
       <c r="Q20" t="n">
-        <v>3.616667046638094e-08</v>
+        <v>3.674993018030371e-08</v>
       </c>
       <c r="R20" t="n">
-        <v>2.017923645205168</v>
+        <v>2.014531483979411</v>
       </c>
       <c r="S20" t="n">
-        <v>4.192526424861096</v>
+        <v>4.196546925598039</v>
       </c>
       <c r="T20" t="n">
-        <v>0.02476113872141749</v>
+        <v>0.02480769349629693</v>
       </c>
       <c r="U20" t="n">
-        <v>2.085550667817387</v>
+        <v>2.085492355303519</v>
       </c>
       <c r="V20" t="n">
-        <v>1.188447022390445e-08</v>
+        <v>1.188559252519676e-08</v>
       </c>
       <c r="W20" t="n">
-        <v>9.915521952990999e-05</v>
+        <v>9.920694619956655e-05</v>
       </c>
     </row>
     <row r="21">
@@ -1861,16 +1861,16 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>887314</v>
+        <v>887174</v>
       </c>
       <c r="E21" t="n">
-        <v>4509200</v>
+        <v>4517998</v>
       </c>
       <c r="F21" t="n">
-        <v>1592.34</v>
+        <v>1595.29</v>
       </c>
       <c r="G21" t="n">
-        <v>20</v>
+        <v>19.79</v>
       </c>
       <c r="H21" t="n">
         <v>0.5</v>
@@ -1897,28 +1897,28 @@
         <v>10</v>
       </c>
       <c r="P21" t="n">
-        <v>0.0008874989721498599</v>
+        <v>0.0008873626933204677</v>
       </c>
       <c r="Q21" t="n">
-        <v>4.03537470213672e-08</v>
+        <v>4.101326744757732e-08</v>
       </c>
       <c r="R21" t="n">
-        <v>2.018890640049732</v>
+        <v>2.015381791628192</v>
       </c>
       <c r="S21" t="n">
-        <v>4.509539216735749</v>
+        <v>4.514552458846584</v>
       </c>
       <c r="T21" t="n">
-        <v>0.02663335035302132</v>
+        <v>0.02668750172640323</v>
       </c>
       <c r="U21" t="n">
-        <v>2.085552778344809</v>
+        <v>2.085494447249077</v>
       </c>
       <c r="V21" t="n">
-        <v>1.327753550876544e-08</v>
+        <v>1.327855766630068e-08</v>
       </c>
       <c r="W21" t="n">
-        <v>0.0001096361443626697</v>
+        <v>0.0001096936629491691</v>
       </c>
     </row>
     <row r="22">
@@ -1936,16 +1936,16 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>984751</v>
+        <v>984585</v>
       </c>
       <c r="E22" t="n">
-        <v>4815910</v>
+        <v>4826330</v>
       </c>
       <c r="F22" t="n">
-        <v>1592.38</v>
+        <v>1595.54</v>
       </c>
       <c r="G22" t="n">
-        <v>20</v>
+        <v>19.79</v>
       </c>
       <c r="H22" t="n">
         <v>0.5</v>
@@ -1972,28 +1972,28 @@
         <v>10</v>
       </c>
       <c r="P22" t="n">
-        <v>0.0009849560644927973</v>
+        <v>0.0009847940822291213</v>
       </c>
       <c r="Q22" t="n">
-        <v>4.451115156572254e-08</v>
+        <v>4.524690787590337e-08</v>
       </c>
       <c r="R22" t="n">
-        <v>2.019718258716352</v>
+        <v>2.016109853709128</v>
       </c>
       <c r="S22" t="n">
-        <v>4.816271269468879</v>
+        <v>4.822647610700759</v>
       </c>
       <c r="T22" t="n">
-        <v>0.02844486979407193</v>
+        <v>0.02850875113254024</v>
       </c>
       <c r="U22" t="n">
-        <v>2.085553959265336</v>
+        <v>2.085495612408729</v>
       </c>
       <c r="V22" t="n">
-        <v>1.466015613456649e-08</v>
+        <v>1.466127880564669e-08</v>
       </c>
       <c r="W22" t="n">
-        <v>0.0001200232213171737</v>
+        <v>0.0001200896162060546</v>
       </c>
     </row>
     <row r="23">
@@ -2011,16 +2011,16 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="E23" t="n">
-        <v>-15</v>
+        <v>-25</v>
       </c>
       <c r="F23" t="n">
-        <v>1591.67</v>
+        <v>1594.71</v>
       </c>
       <c r="G23" t="n">
-        <v>20</v>
+        <v>19.77</v>
       </c>
       <c r="H23" t="n">
         <v>0.5</v>
@@ -2065,10 +2065,10 @@
         <v>0</v>
       </c>
       <c r="V23" t="n">
-        <v>1.256541871518141e-09</v>
+        <v>1.254146522890935e-09</v>
       </c>
       <c r="W23" t="n">
-        <v>1.25654187145124e-05</v>
+        <v>1.254146522785571e-05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>